<commit_message>
Two books added to the list
</commit_message>
<xml_diff>
--- a/Venukumar_Books List .xlsx
+++ b/Venukumar_Books List .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Books\My Books List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43006A6E-C362-4E74-A1B3-24E134694128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EA1F2B-6CE9-4DC3-8CBD-F10E034C8C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6C2F08D3-1046-4AA4-870F-D6A612D769D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="103">
   <si>
     <t>#</t>
   </si>
@@ -334,6 +334,15 @@
   </si>
   <si>
     <t>Chitra Banerjee</t>
+  </si>
+  <si>
+    <t>Wish I could Tell You</t>
+  </si>
+  <si>
+    <t>My Father Baliah</t>
+  </si>
+  <si>
+    <t>Satyanarayana Y B</t>
   </si>
 </sst>
 </file>
@@ -431,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -443,9 +452,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -774,20 +780,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A302F8-F52A-450D-BD5D-7B6EE8B1BDAE}">
-  <dimension ref="E4:H55"/>
+  <dimension ref="E4:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="9.140625" style="6"/>
-    <col min="5" max="5" width="4.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="60" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="4" width="9.140625" style="5"/>
+    <col min="5" max="5" width="4.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="4" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
@@ -808,7 +814,7 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -822,7 +828,7 @@
       <c r="E6" s="2">
         <v>2</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -836,7 +842,7 @@
       <c r="E7" s="2">
         <v>3</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -850,7 +856,7 @@
       <c r="E8" s="2">
         <v>4</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -864,7 +870,7 @@
       <c r="E9" s="2">
         <v>5</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -878,7 +884,7 @@
       <c r="E10" s="2">
         <v>6</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
@@ -892,7 +898,7 @@
       <c r="E11" s="2">
         <v>7</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -906,7 +912,7 @@
       <c r="E12" s="2">
         <v>8</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>21</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -920,7 +926,7 @@
       <c r="E13" s="2">
         <v>9</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -934,7 +940,7 @@
       <c r="E14" s="2">
         <v>10</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -948,7 +954,7 @@
       <c r="E15" s="2">
         <v>11</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>27</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -962,7 +968,7 @@
       <c r="E16" s="2">
         <v>12</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>29</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -976,7 +982,7 @@
       <c r="E17" s="2">
         <v>13</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="7" t="s">
         <v>31</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -990,7 +996,7 @@
       <c r="E18" s="2">
         <v>14</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>33</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1004,7 +1010,7 @@
       <c r="E19" s="2">
         <v>15</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="7" t="s">
         <v>35</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -1018,7 +1024,7 @@
       <c r="E20" s="2">
         <v>16</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1032,7 +1038,7 @@
       <c r="E21" s="2">
         <v>17</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>40</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -1046,7 +1052,7 @@
       <c r="E22" s="2">
         <v>18</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -1060,7 +1066,7 @@
       <c r="E23" s="2">
         <v>19</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>43</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -1074,7 +1080,7 @@
       <c r="E24" s="2">
         <v>20</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="7" t="s">
         <v>44</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -1088,7 +1094,7 @@
       <c r="E25" s="2">
         <v>21</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -1102,7 +1108,7 @@
       <c r="E26" s="2">
         <v>22</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>47</v>
       </c>
       <c r="G26" s="3" t="s">
@@ -1116,7 +1122,7 @@
       <c r="E27" s="2">
         <v>23</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="7" t="s">
         <v>49</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -1130,7 +1136,7 @@
       <c r="E28" s="2">
         <v>24</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="7" t="s">
         <v>50</v>
       </c>
       <c r="G28" s="3" t="s">
@@ -1144,7 +1150,7 @@
       <c r="E29" s="2">
         <v>25</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="7" t="s">
         <v>52</v>
       </c>
       <c r="G29" s="3" t="s">
@@ -1158,7 +1164,7 @@
       <c r="E30" s="2">
         <v>26</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="7" t="s">
         <v>55</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -1172,7 +1178,7 @@
       <c r="E31" s="2">
         <v>27</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="7" t="s">
         <v>57</v>
       </c>
       <c r="G31" s="3" t="s">
@@ -1186,7 +1192,7 @@
       <c r="E32" s="2">
         <v>28</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="7" t="s">
         <v>58</v>
       </c>
       <c r="G32" s="3" t="s">
@@ -1200,7 +1206,7 @@
       <c r="E33" s="2">
         <v>29</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F33" s="7" t="s">
         <v>61</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -1214,7 +1220,7 @@
       <c r="E34" s="2">
         <v>30</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="7" t="s">
         <v>62</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -1228,7 +1234,7 @@
       <c r="E35" s="2">
         <v>31</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="7" t="s">
         <v>64</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -1242,7 +1248,7 @@
       <c r="E36" s="2">
         <v>32</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="7" t="s">
         <v>66</v>
       </c>
       <c r="G36" s="3" t="s">
@@ -1256,7 +1262,7 @@
       <c r="E37" s="2">
         <v>33</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F37" s="7" t="s">
         <v>67</v>
       </c>
       <c r="G37" s="3" t="s">
@@ -1270,7 +1276,7 @@
       <c r="E38" s="2">
         <v>34</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F38" s="7" t="s">
         <v>69</v>
       </c>
       <c r="G38" s="3" t="s">
@@ -1284,7 +1290,7 @@
       <c r="E39" s="2">
         <v>35</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F39" s="7" t="s">
         <v>72</v>
       </c>
       <c r="G39" s="3" t="s">
@@ -1298,7 +1304,7 @@
       <c r="E40" s="2">
         <v>36</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F40" s="7" t="s">
         <v>74</v>
       </c>
       <c r="G40" s="3" t="s">
@@ -1312,7 +1318,7 @@
       <c r="E41" s="2">
         <v>37</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F41" s="7" t="s">
         <v>76</v>
       </c>
       <c r="G41" s="3" t="s">
@@ -1326,7 +1332,7 @@
       <c r="E42" s="2">
         <v>38</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F42" s="7" t="s">
         <v>79</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -1340,7 +1346,7 @@
       <c r="E43" s="2">
         <v>39</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="7" t="s">
         <v>80</v>
       </c>
       <c r="G43" s="3" t="s">
@@ -1354,7 +1360,7 @@
       <c r="E44" s="2">
         <v>40</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F44" s="7" t="s">
         <v>81</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -1368,7 +1374,7 @@
       <c r="E45" s="2">
         <v>41</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F45" s="7" t="s">
         <v>82</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -1382,7 +1388,7 @@
       <c r="E46" s="2">
         <v>42</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F46" s="7" t="s">
         <v>83</v>
       </c>
       <c r="G46" s="3" t="s">
@@ -1396,7 +1402,7 @@
       <c r="E47" s="2">
         <v>43</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F47" s="7" t="s">
         <v>85</v>
       </c>
       <c r="G47" s="3" t="s">
@@ -1410,7 +1416,7 @@
       <c r="E48" s="2">
         <v>44</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F48" s="7" t="s">
         <v>87</v>
       </c>
       <c r="G48" s="3" t="s">
@@ -1424,7 +1430,7 @@
       <c r="E49" s="2">
         <v>45</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F49" s="7" t="s">
         <v>89</v>
       </c>
       <c r="G49" s="3" t="s">
@@ -1438,7 +1444,7 @@
       <c r="E50" s="2">
         <v>46</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F50" s="7" t="s">
         <v>90</v>
       </c>
       <c r="G50" s="3" t="s">
@@ -1452,7 +1458,7 @@
       <c r="E51" s="2">
         <v>47</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F51" s="7" t="s">
         <v>92</v>
       </c>
       <c r="G51" s="3" t="s">
@@ -1466,7 +1472,7 @@
       <c r="E52" s="2">
         <v>48</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F52" s="7" t="s">
         <v>94</v>
       </c>
       <c r="G52" s="3" t="s">
@@ -1480,7 +1486,7 @@
       <c r="E53" s="2">
         <v>49</v>
       </c>
-      <c r="F53" s="8" t="s">
+      <c r="F53" s="7" t="s">
         <v>95</v>
       </c>
       <c r="G53" s="3" t="s">
@@ -1494,7 +1500,7 @@
       <c r="E54" s="2">
         <v>50</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F54" s="7" t="s">
         <v>98</v>
       </c>
       <c r="G54" s="3" t="s">
@@ -1505,10 +1511,32 @@
       </c>
     </row>
     <row r="55" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
+      <c r="E55" s="2">
+        <v>51</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="5:8" ht="21" x14ac:dyDescent="0.55000000000000004">
+      <c r="E56" s="2">
+        <v>52</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>